<commit_message>
crtypt and decrypt 2
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fikri\Api\testApi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Diri\Belajar\Java\ApiTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD933E9-94E2-46D2-A98A-A751367AD681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60DB4D4-CAF3-4E60-8F3C-463239923870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{923F321B-0599-4186-96E6-5E2452019B8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{923F321B-0599-4186-96E6-5E2452019B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="credential" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,25 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>fikri</t>
-  </si>
-  <si>
-    <t>fikri123</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>tulisan 1</t>
-  </si>
-  <si>
-    <t>tulisan 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>203ec648ad2d51c5faff8a6ef1869d4300936d762434843a3697aaed81e57081</t>
   </si>
@@ -81,13 +63,24 @@
   </si>
   <si>
     <t>newuser</t>
+  </si>
+  <si>
+    <t>q7SoVpPm1QWzVifxqyXRog==</t>
+  </si>
+  <si>
+    <t>usere2e</t>
+  </si>
+  <si>
+    <t>secret</t>
+  </si>
+  <si>
+    <t>AutomationChannellingKeySecret</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,85 +433,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0C68D2-ABB6-4593-87E4-D493B754247D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="69.28125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.01953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="69.28125" collapsed="true"/>
+    <col min="2" max="2" width="69.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="69.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GVg0EcPsj699bHaGi1Gkh5KQStUqSdTwrH0I0D05P8U3hjPJMx8EFKIt2chcnYt1JTmFv+mbyg4nCl3UrFGglw==" saltValue="dke1XTIv9E6WBzyBaVvj9w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="s0bIFsm4jzJai3+158/Axo4hqYuax/Bojuwzibn4HHFRUNdlUdJ/vffo8YtX68FHxYarsmnLyXAExPnbxadDcA==" saltValue="HAh++9R4w37b2SwyzIr3TA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>